<commit_message>
Added energy terms which are probably useless
</commit_message>
<xml_diff>
--- a/src/vectors.xlsx
+++ b/src/vectors.xlsx
@@ -373,552 +373,552 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>-0.5773502691896257</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>-0.5773502691896257</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>-0.5773502691896257</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>0.5178665886597253</v>
+        <v>-0.00038742819433336596</v>
       </c>
       <c r="B3">
-        <v>0.5786462339034713</v>
+        <v>-0.06479935270847112</v>
       </c>
       <c r="C3">
-        <v>0.6300656571654005</v>
+        <v>0.9978982381926312</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>-0.4568793676883185</v>
+        <v>0.0007653948946984158</v>
       </c>
       <c r="B4">
-        <v>-0.5763996891364502</v>
+        <v>0.12801546965896227</v>
       </c>
       <c r="C4">
-        <v>-0.6775135731069347</v>
+        <v>-0.9917718758356936</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>0.3897700724682307</v>
+        <v>-0.0011555889232988086</v>
       </c>
       <c r="B5">
-        <v>0.57031782729293</v>
+        <v>-0.19327813143520226</v>
       </c>
       <c r="C5">
-        <v>0.7230607626472217</v>
+        <v>0.9811433272071707</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>-0.32576404553160276</v>
+        <v>0.001517954998238078</v>
       </c>
       <c r="B6">
-        <v>-0.5613926755535539</v>
+        <v>0.25388421980753506</v>
       </c>
       <c r="C6">
-        <v>-0.7607338893947778</v>
+        <v>-0.9672334251592749</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>0.2528774014275434</v>
+        <v>-0.001903814559868042</v>
       </c>
       <c r="B7">
-        <v>0.5478680514417034</v>
+        <v>-0.31842254037326667</v>
       </c>
       <c r="C7">
-        <v>0.7974293812349305</v>
+        <v>0.9479469717617948</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>-0.18800257854746064</v>
+        <v>0.002245110873152343</v>
       </c>
       <c r="B8">
-        <v>-0.533039055323284</v>
+        <v>0.3755039216889036</v>
       </c>
       <c r="C8">
-        <v>-0.824939025601024</v>
+        <v>-0.9268180858579643</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>0.11152107305442623</v>
+        <v>-0.0026193129364291043</v>
       </c>
       <c r="B9">
-        <v>0.5123723152329317</v>
+        <v>-0.43809296220881694</v>
       </c>
       <c r="C9">
-        <v>0.8514914332203435</v>
+        <v>0.8989258565993332</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>-0.04778552906679614</v>
+        <v>0.002934810274066609</v>
       </c>
       <c r="B10">
-        <v>-0.49261285386736037</v>
+        <v>0.490858766041759</v>
       </c>
       <c r="C10">
-        <v>-0.8689356244374269</v>
+        <v>-0.8712342157471875</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>-0.029956668827330415</v>
+        <v>-0.0032900104100215817</v>
       </c>
       <c r="B11">
-        <v>0.46545181326888674</v>
+        <v>-0.5502699842317609</v>
       </c>
       <c r="C11">
-        <v>0.884566112575807</v>
+        <v>0.8349803113158295</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>0.09082850580813866</v>
+        <v>0.003575744673273488</v>
       </c>
       <c r="B12">
-        <v>-0.4418433165895283</v>
+        <v>0.598057355371699</v>
       </c>
       <c r="C12">
-        <v>-0.8924823057729643</v>
+        <v>-0.8014453279768001</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>-0.16754523217317518</v>
+        <v>-0.003904786289461346</v>
       </c>
       <c r="B13">
-        <v>0.4091154340232017</v>
+        <v>-0.6530936127410855</v>
       </c>
       <c r="C13">
-        <v>0.8969688717118584</v>
+        <v>0.7572671164396554</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>0.22420930898693922</v>
+        <v>0.004157541817403305</v>
       </c>
       <c r="B14">
-        <v>-0.3827484378288104</v>
+        <v>0.6953649111688653</v>
       </c>
       <c r="C14">
-        <v>-0.8962331276532933</v>
+        <v>-0.7186448045878802</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>-0.2978386038961743</v>
+        <v>-0.004453662147187283</v>
       </c>
       <c r="B15">
-        <v>0.34556138256936225</v>
+        <v>-0.7448949370092951</v>
       </c>
       <c r="C15">
-        <v>0.8898761132348304</v>
+        <v>0.6671669189276377</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>0.34936870960843014</v>
+        <v>0.004670919699352832</v>
       </c>
       <c r="B16">
-        <v>-0.31744721154015576</v>
+        <v>0.7812290238136452</v>
       </c>
       <c r="C16">
-        <v>-0.8815717626103504</v>
+        <v>-0.6242270379119613</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>-0.4181958472185164</v>
+        <v>-0.004927942843629012</v>
       </c>
       <c r="B17">
-        <v>0.27698040984030414</v>
+        <v>-0.824219712269636</v>
       </c>
       <c r="C17">
-        <v>0.8650977320129123</v>
+        <v>0.5662486920828059</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>0.4640635014151477</v>
+        <v>0.005107801621124121</v>
       </c>
       <c r="B18">
-        <v>-0.24798742858705963</v>
+        <v>0.8542988912838118</v>
       </c>
       <c r="C18">
-        <v>-0.8503806805878714</v>
+        <v>-0.5197569765898763</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>-0.5267789642442589</v>
+        <v>-0.005320311079320032</v>
       </c>
       <c r="B19">
-        <v>0.20539543629258156</v>
+        <v>-0.8898441660352499</v>
       </c>
       <c r="C19">
-        <v>0.8248130925124345</v>
+        <v>0.45623355253975995</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>0.5667897374266612</v>
+        <v>0.005461395919315531</v>
       </c>
       <c r="B20">
-        <v>-0.17621575971465475</v>
+        <v>0.9134386449448185</v>
       </c>
       <c r="C20">
-        <v>-0.8047964957528103</v>
+        <v>-0.4069398175111232</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>-0.6224872660928809</v>
+        <v>-0.005624881440795569</v>
       </c>
       <c r="B21">
-        <v>0.13255694886336866</v>
+        <v>-0.9407840268366269</v>
       </c>
       <c r="C21">
-        <v>0.7713224091521296</v>
+        <v>0.33895984357713776</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>0.6566930282789057</v>
+        <v>0.005726246888487177</v>
       </c>
       <c r="B22">
-        <v>-0.10370192423103036</v>
+        <v>0.9577358567432487</v>
       </c>
       <c r="C22">
-        <v>-0.7469940947026702</v>
+        <v>-0.2875921396784821</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>-0.7048238371969809</v>
+        <v>-0.005837222709232087</v>
       </c>
       <c r="B23">
-        <v>0.05989714661379542</v>
+        <v>-0.9762982435890242</v>
       </c>
       <c r="C23">
-        <v>0.7068491284188226</v>
+        <v>0.21635079476634533</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>0.7334294536406145</v>
+        <v>0.005898265112868237</v>
       </c>
       <c r="B24">
-        <v>-0.03171504821244698</v>
+        <v>0.9865066025052299</v>
       </c>
       <c r="C24">
-        <v>-0.679025325189946</v>
+        <v>-0.16361520003424695</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>-0.7737322828325653</v>
+        <v>-0.005954358401337208</v>
       </c>
       <c r="B25">
-        <v>-0.011466202989531691</v>
+        <v>-0.9958890646860539</v>
       </c>
       <c r="C25">
-        <v>0.6334089363844735</v>
+        <v>0.09038537743885801</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>0.7970104194729434</v>
+        <v>0.0059747456582586855</v>
       </c>
       <c r="B26">
-        <v>0.038758516840837226</v>
+        <v>0.9992984963957261</v>
       </c>
       <c r="C26">
-        <v>-0.6027206389562758</v>
+        <v>-0.036970495203068214</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>-0.8294350264688957</v>
+        <v>-0.005974755110647236</v>
       </c>
       <c r="B27">
-        <v>-0.08069100093496374</v>
+        <v>-0.9993000786464137</v>
       </c>
       <c r="C27">
-        <v>0.5527445153365668</v>
+        <v>-0.03692770123686471</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28">
-        <v>0.8476568751075167</v>
+        <v>0.005954381438418042</v>
       </c>
       <c r="B28">
-        <v>0.10697002180522541</v>
+        <v>0.9958929211186931</v>
       </c>
       <c r="C28">
-        <v>-0.5196491475196986</v>
+        <v>0.09034287469060583</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>-0.8722937039637594</v>
+        <v>-0.005898306426805656</v>
       </c>
       <c r="B29">
-        <v>-0.14715244915802153</v>
+        <v>-0.9865135183259799</v>
       </c>
       <c r="C29">
-        <v>0.4663151838960221</v>
+        <v>-0.1635734946175323</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>0.885678557705397</v>
+        <v>0.0058372767756569915</v>
       </c>
       <c r="B30">
-        <v>0.1723492289004264</v>
+        <v>0.9763072942847668</v>
       </c>
       <c r="C30">
-        <v>-0.43112554519341106</v>
+        <v>0.21630994735841966</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>-0.9027020685606926</v>
+        <v>-0.005726317393330945</v>
       </c>
       <c r="B31">
-        <v>-0.2103778109015306</v>
+        <v>-0.957747659074566</v>
       </c>
       <c r="C31">
-        <v>0.3753267271278808</v>
+        <v>-0.28755283136547244</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>0.9113855579423065</v>
+        <v>0.005624963070010575</v>
       </c>
       <c r="B32">
-        <v>0.2344421169289831</v>
+        <v>0.9407976915035984</v>
       </c>
       <c r="C32">
-        <v>-0.33825028985064853</v>
+        <v>0.33892191350215356</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>-0.9210144217886864</v>
+        <v>-0.005461491070674445</v>
       </c>
       <c r="B33">
-        <v>-0.26998346947067675</v>
+        <v>-0.913454573066334</v>
       </c>
       <c r="C33">
-        <v>0.28078703864286164</v>
+        <v>-0.4069040612472263</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
-        <v>0.9250337745697627</v>
+        <v>0.005320415004345975</v>
       </c>
       <c r="B34">
-        <v>0.29285297672637106</v>
+        <v>0.8898615629933536</v>
       </c>
       <c r="C34">
-        <v>-0.24197034927387523</v>
+        <v>0.45619961846894086</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>-0.9275082287715892</v>
+        <v>-0.00510791528450765</v>
       </c>
       <c r="B35">
-        <v>-0.32562024346322593</v>
+        <v>-0.8543179182957685</v>
       </c>
       <c r="C35">
-        <v>0.18357544118955213</v>
+        <v>-0.5197257004230508</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>0.9268026281446807</v>
+        <v>0.004928062318662813</v>
       </c>
       <c r="B36">
-        <v>0.3471959123287061</v>
+        <v>0.8242397122846975</v>
       </c>
       <c r="C36">
-        <v>-0.14314987574689075</v>
+        <v>0.5662195783392008</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37">
-        <v>-0.922377548675682</v>
+        <v>-0.0046710445338058555</v>
       </c>
       <c r="B37">
-        <v>-0.3769306160917248</v>
+        <v>-0.7812499208555906</v>
       </c>
       <c r="C37">
-        <v>0.08451608339098936</v>
+        <v>-0.6242008831346657</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38">
-        <v>0.9168019284766532</v>
+        <v>0.004453789369298145</v>
       </c>
       <c r="B38">
-        <v>0.39705902999192894</v>
+        <v>0.7449162338831113</v>
       </c>
       <c r="C38">
-        <v>-0.04264212287584127</v>
+        <v>0.667143139256978</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>-0.9057531722196177</v>
+        <v>-0.004157669738647154</v>
       </c>
       <c r="B39">
-        <v>-0.423520150992469</v>
+        <v>-0.6953863249476983</v>
       </c>
       <c r="C39">
-        <v>-0.015552257630831097</v>
+        <v>-0.7186240831325362</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40">
-        <v>0.8951040743940926</v>
+        <v>0.0039049128978508986</v>
       </c>
       <c r="B40">
-        <v>0.44198357759461737</v>
+        <v>0.653114806886069</v>
       </c>
       <c r="C40">
-        <v>0.058644804882938356</v>
+        <v>0.757248836698633</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
-        <v>-0.8777449573958246</v>
+        <v>-0.0035758673702375792</v>
       </c>
       <c r="B41">
-        <v>-0.4649445897807483</v>
+        <v>-0.5980778946276303</v>
       </c>
       <c r="C41">
-        <v>-0.11571654246396146</v>
+        <v>-0.8014300001437002</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42">
-        <v>0.8617970000616396</v>
+        <v>0.0032901280334741217</v>
       </c>
       <c r="B42">
-        <v>0.48145963004532155</v>
+        <v>0.5502896743132761</v>
       </c>
       <c r="C42">
-        <v>0.15969519504788046</v>
+        <v>0.8349673343321353</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43">
-        <v>-0.8385011261826343</v>
+        <v>-0.0029349197477157862</v>
       </c>
       <c r="B43">
-        <v>-0.5007135294031082</v>
+        <v>-0.49087709174710326</v>
       </c>
       <c r="C43">
-        <v>-0.21494609292363673</v>
+        <v>-0.8712238903083296</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44">
-        <v>0.817051974227904</v>
+        <v>0.002619413753734472</v>
       </c>
       <c r="B44">
-        <v>0.5149391674870332</v>
+        <v>0.43810983895991</v>
       </c>
       <c r="C44">
-        <v>0.2593525114550573</v>
+        <v>0.8989176311977135</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45">
-        <v>-0.7882779362681468</v>
+        <v>-0.0022451999629197385</v>
       </c>
       <c r="B45">
-        <v>-0.5303107433463208</v>
+        <v>-0.37551883517264256</v>
       </c>
       <c r="C45">
-        <v>-0.31207116285280884</v>
+        <v>-0.9268120432470157</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46">
-        <v>0.761198418906766</v>
+        <v>0.0019038918341658597</v>
       </c>
       <c r="B46">
-        <v>0.5418661812917946</v>
+        <v>0.31843547604452427</v>
       </c>
       <c r="C46">
-        <v>0.3563116734350528</v>
+        <v>0.9479426263187983</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47">
-        <v>-0.7275112984553486</v>
+        <v>-0.001518017859968651</v>
       </c>
       <c r="B47">
-        <v>-0.5532298444532102</v>
+        <v>-0.25389474276327534</v>
       </c>
       <c r="C47">
-        <v>-0.40578818344807627</v>
+        <v>-0.9672306628818934</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48">
-        <v>0.6947957127495477</v>
+        <v>0.001155637470468096</v>
       </c>
       <c r="B48">
-        <v>0.5617215658527447</v>
+        <v>0.19328625820424777</v>
       </c>
       <c r="C48">
-        <v>0.449141180477574</v>
+        <v>0.981141726200368</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49">
-        <v>-0.6568801184666032</v>
+        <v>-0.000765427395482992</v>
       </c>
       <c r="B49">
-        <v>-0.5690220217297306</v>
+        <v>-0.12802091024066778</v>
       </c>
       <c r="C49">
-        <v>-0.494694298279161</v>
+        <v>-0.9917711735385604</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50">
-        <v>0.6186902818785246</v>
+        <v>0.0003874447484656346</v>
       </c>
       <c r="B50">
-        <v>0.5740781107937165</v>
+        <v>0.06480212386131848</v>
       </c>
       <c r="C50">
-        <v>0.5363363290106212</v>
+        <v>0.9978980582352233</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51">
-        <v>-0.5773502691896257</v>
+        <v>-0</v>
       </c>
       <c r="B51">
-        <v>-0.5773502691896257</v>
+        <v>-0</v>
       </c>
       <c r="C51">
-        <v>-0.5773502691896257</v>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>